<commit_message>
Inclusão do diagrama de casos de uso
</commit_message>
<xml_diff>
--- a/Requisitos e Casos de Uso.xlsx
+++ b/Requisitos e Casos de Uso.xlsx
@@ -125,9 +125,6 @@
     <t>Consultar Soluções</t>
   </si>
   <si>
-    <t>Disponibilizar Solução</t>
-  </si>
-  <si>
     <t>Usuário, Assinante, Professor</t>
   </si>
   <si>
@@ -171,6 +168,9 @@
   </si>
   <si>
     <t>Logar no Sistema</t>
+  </si>
+  <si>
+    <t>Consultar Problemas</t>
   </si>
 </sst>
 </file>
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +567,7 @@
         <v>3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -580,17 +580,15 @@
       <c r="C3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="4">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>33</v>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
-        <v>33</v>
+      <c r="H3" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -603,9 +601,7 @@
       <c r="C4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="4">
-        <v>2</v>
-      </c>
+      <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
         <v>6</v>
       </c>
@@ -626,9 +622,7 @@
       <c r="C5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="4">
-        <v>3</v>
-      </c>
+      <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
         <v>25</v>
       </c>
@@ -649,9 +643,6 @@
       <c r="C6" t="s">
         <v>26</v>
       </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
       <c r="F6" t="s">
         <v>25</v>
       </c>
@@ -672,9 +663,6 @@
       <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
       <c r="F7" t="s">
         <v>27</v>
       </c>
@@ -695,9 +683,7 @@
       <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="4">
-        <v>6</v>
-      </c>
+      <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
         <v>29</v>
       </c>
@@ -718,9 +704,7 @@
       <c r="C9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="4">
-        <v>7</v>
-      </c>
+      <c r="E9" s="4"/>
       <c r="F9" s="4" t="s">
         <v>30</v>
       </c>
@@ -728,7 +712,7 @@
         <v>7</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -741,9 +725,7 @@
       <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="4">
-        <v>8</v>
-      </c>
+      <c r="E10" s="4"/>
       <c r="F10" s="4" t="s">
         <v>31</v>
       </c>
@@ -764,9 +746,7 @@
       <c r="C11" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="4">
-        <v>9</v>
-      </c>
+      <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
         <v>6</v>
       </c>
@@ -774,7 +754,7 @@
         <v>9</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -785,19 +765,17 @@
         <v>14</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="4">
-        <v>10</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="4">
         <v>10</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -810,17 +788,15 @@
       <c r="C13" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="4">
-        <v>11</v>
-      </c>
+      <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="4">
         <v>11</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -833,17 +809,15 @@
       <c r="C14" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="4">
         <v>12</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14">
-        <v>12</v>
-      </c>
       <c r="H14" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -856,17 +830,15 @@
       <c r="C15" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="4"/>
+      <c r="F15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="4">
         <v>13</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15">
-        <v>13</v>
-      </c>
       <c r="H15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -879,17 +851,15 @@
       <c r="C16" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="4">
         <v>14</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16">
-        <v>14</v>
-      </c>
       <c r="H16" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -902,17 +872,15 @@
       <c r="C17" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="4">
-        <v>15</v>
-      </c>
+      <c r="E17" s="4"/>
       <c r="F17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="4">
         <v>15</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -923,15 +891,13 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="4">
-        <v>16</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18">
+      <c r="G18" s="4">
         <v>16</v>
       </c>
       <c r="H18" s="4" t="s">
@@ -946,13 +912,11 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="4">
-        <v>17</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E19" s="4"/>
       <c r="F19" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -965,11 +929,9 @@
       <c r="C20" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="4">
-        <v>18</v>
-      </c>
+      <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>